<commit_message>
boston, birmingham, cleveland and columbus
</commit_message>
<xml_diff>
--- a/data/input_data_US_Boston.xlsx
+++ b/data/input_data_US_Boston.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anna.palmer\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB226DF-D0CA-47DF-BCE4-32BF536BEABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62F75B4-D915-4D8C-BA19-F16DC8AECFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14610" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14610" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="101">
   <si>
     <t>0-4</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>days_changed</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Columbus</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,12 +432,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -768,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -888,24 +888,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -926,6 +908,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,7 +1364,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="81" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1421,7 +1424,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1479,7 +1482,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="81" t="s">
         <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1555,7 +1558,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1632,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="81" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="48" t="s">
@@ -1689,7 +1692,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="48" t="s">
         <v>20</v>
       </c>
@@ -1747,7 +1750,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="81" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -1823,7 +1826,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="70"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="48" t="s">
         <v>21</v>
       </c>
@@ -1896,84 +1899,636 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="47">
+        <v>11294</v>
+      </c>
+      <c r="D10" s="47">
+        <v>12657</v>
+      </c>
+      <c r="E10" s="47">
+        <v>9864</v>
+      </c>
+      <c r="F10" s="47">
+        <v>11603</v>
+      </c>
+      <c r="G10" s="47">
+        <v>15089</v>
+      </c>
+      <c r="H10" s="47">
+        <v>17383</v>
+      </c>
+      <c r="I10" s="47">
+        <v>14409</v>
+      </c>
+      <c r="J10" s="47">
+        <v>10626</v>
+      </c>
+      <c r="K10" s="47">
+        <v>9934</v>
+      </c>
+      <c r="L10" s="47">
+        <v>11297</v>
+      </c>
+      <c r="M10" s="47">
+        <v>12876</v>
+      </c>
+      <c r="N10" s="47">
+        <v>14713</v>
+      </c>
+      <c r="O10" s="47">
+        <v>12912</v>
+      </c>
+      <c r="P10" s="47">
+        <v>10163</v>
+      </c>
+      <c r="Q10" s="47">
+        <v>7064</v>
+      </c>
+      <c r="R10" s="47">
+        <v>13416</v>
+      </c>
+      <c r="S10" s="47">
+        <f>SUM(C10:R10)</f>
+        <v>195300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A11" s="81"/>
+      <c r="B11" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="47">
+        <v>12550</v>
+      </c>
+      <c r="D11" s="47">
+        <v>8948</v>
+      </c>
+      <c r="E11" s="47">
+        <v>12505</v>
+      </c>
+      <c r="F11" s="47">
+        <v>12851</v>
+      </c>
+      <c r="G11" s="47">
+        <v>15438</v>
+      </c>
+      <c r="H11" s="47">
+        <v>17098</v>
+      </c>
+      <c r="I11" s="47">
+        <v>13838</v>
+      </c>
+      <c r="J11" s="47">
+        <v>11521</v>
+      </c>
+      <c r="K11" s="47">
+        <v>10452</v>
+      </c>
+      <c r="L11" s="47">
+        <v>9906</v>
+      </c>
+      <c r="M11" s="47">
+        <v>11526</v>
+      </c>
+      <c r="N11" s="47">
+        <v>14819</v>
+      </c>
+      <c r="O11" s="47">
+        <v>12937</v>
+      </c>
+      <c r="P11" s="47">
+        <v>8989</v>
+      </c>
+      <c r="Q11" s="47">
+        <v>6439</v>
+      </c>
+      <c r="R11" s="47">
+        <v>8664</v>
+      </c>
+      <c r="S11" s="47">
+        <f>SUM(C11:R11)</f>
+        <v>188481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A12" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="47">
+        <f t="shared" ref="C12:S12" si="3">SUM(C10:C11)</f>
+        <v>23844</v>
+      </c>
+      <c r="D12" s="47">
+        <f t="shared" si="3"/>
+        <v>21605</v>
+      </c>
+      <c r="E12" s="47">
+        <f t="shared" si="3"/>
+        <v>22369</v>
+      </c>
+      <c r="F12" s="47">
+        <f t="shared" si="3"/>
+        <v>24454</v>
+      </c>
+      <c r="G12" s="47">
+        <f t="shared" si="3"/>
+        <v>30527</v>
+      </c>
+      <c r="H12" s="47">
+        <f t="shared" si="3"/>
+        <v>34481</v>
+      </c>
+      <c r="I12" s="47">
+        <f t="shared" si="3"/>
+        <v>28247</v>
+      </c>
+      <c r="J12" s="47">
+        <f t="shared" si="3"/>
+        <v>22147</v>
+      </c>
+      <c r="K12" s="47">
+        <f t="shared" si="3"/>
+        <v>20386</v>
+      </c>
+      <c r="L12" s="47">
+        <f t="shared" si="3"/>
+        <v>21203</v>
+      </c>
+      <c r="M12" s="47">
+        <f t="shared" si="3"/>
+        <v>24402</v>
+      </c>
+      <c r="N12" s="47">
+        <f t="shared" si="3"/>
+        <v>29532</v>
+      </c>
+      <c r="O12" s="47">
+        <f t="shared" si="3"/>
+        <v>25849</v>
+      </c>
+      <c r="P12" s="47">
+        <f t="shared" si="3"/>
+        <v>19152</v>
+      </c>
+      <c r="Q12" s="47">
+        <f t="shared" si="3"/>
+        <v>13503</v>
+      </c>
+      <c r="R12" s="47">
+        <f t="shared" si="3"/>
+        <v>22080</v>
+      </c>
+      <c r="S12" s="47">
+        <f t="shared" si="3"/>
+        <v>383781</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A13" s="81"/>
+      <c r="B13" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <f>C12/S12</f>
+        <v>6.2129183049708034E-2</v>
+      </c>
+      <c r="D13">
+        <f>D12/S12</f>
+        <v>5.6295126647749626E-2</v>
+      </c>
+      <c r="E13">
+        <f>E12/S12</f>
+        <v>5.8285845312821633E-2</v>
+      </c>
+      <c r="F13">
+        <f>F12/S12</f>
+        <v>6.3718631198522072E-2</v>
+      </c>
+      <c r="G13">
+        <f>G12/S12</f>
+        <v>7.9542760063682147E-2</v>
+      </c>
+      <c r="H13">
+        <f>H12/S12</f>
+        <v>8.9845510851240679E-2</v>
+      </c>
+      <c r="I13">
+        <f>I12/S12</f>
+        <v>7.3601871900901811E-2</v>
+      </c>
+      <c r="J13">
+        <f>J12/S12</f>
+        <v>5.7707390412761447E-2</v>
+      </c>
+      <c r="K13">
+        <f>K12/S12</f>
+        <v>5.3118836002824528E-2</v>
+      </c>
+      <c r="L13">
+        <f>L12/S12</f>
+        <v>5.5247654261154147E-2</v>
+      </c>
+      <c r="M13">
+        <f>M12/S12</f>
+        <v>6.3583137257967437E-2</v>
+      </c>
+      <c r="N13">
+        <f>N12/S12</f>
+        <v>7.695013562422319E-2</v>
+      </c>
+      <c r="O13">
+        <f>O12/S12</f>
+        <v>6.7353516719170572E-2</v>
+      </c>
+      <c r="P13">
+        <f>P12/S12</f>
+        <v>4.990346056735482E-2</v>
+      </c>
+      <c r="Q13">
+        <f>Q12/S12</f>
+        <v>3.5184128448255643E-2</v>
+      </c>
+      <c r="R13">
+        <f>R12/S12</f>
+        <v>5.7532811681662195E-2</v>
+      </c>
+      <c r="S13">
+        <f>S12/S12</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="C14" s="47"/>
+      <c r="A14" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="47">
+        <v>30935</v>
+      </c>
+      <c r="D14" s="47">
+        <v>26456</v>
+      </c>
+      <c r="E14" s="47">
+        <v>24719</v>
+      </c>
+      <c r="F14" s="47">
+        <v>31095</v>
+      </c>
+      <c r="G14" s="47">
+        <v>37110</v>
+      </c>
+      <c r="H14" s="47">
+        <v>52141</v>
+      </c>
+      <c r="I14" s="47">
+        <v>41235</v>
+      </c>
+      <c r="J14" s="47">
+        <v>29921</v>
+      </c>
+      <c r="K14" s="47">
+        <v>28163</v>
+      </c>
+      <c r="L14" s="47">
+        <v>25564</v>
+      </c>
+      <c r="M14" s="47">
+        <v>26006</v>
+      </c>
+      <c r="N14" s="47">
+        <v>23651</v>
+      </c>
+      <c r="O14" s="47">
+        <v>25581</v>
+      </c>
+      <c r="P14" s="47">
+        <v>19552</v>
+      </c>
+      <c r="Q14" s="47">
+        <v>14222</v>
+      </c>
+      <c r="R14" s="47">
+        <v>22313</v>
+      </c>
+      <c r="S14" s="47">
+        <f>SUM(C14:R14)</f>
+        <v>458664</v>
+      </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="C15" s="47"/>
-      <c r="S15" s="47"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="47">
+        <v>33219</v>
+      </c>
+      <c r="D15" s="47">
+        <v>26542</v>
+      </c>
+      <c r="E15" s="47">
+        <v>28311</v>
+      </c>
+      <c r="F15" s="47">
+        <v>30253</v>
+      </c>
+      <c r="G15" s="47">
+        <v>33373</v>
+      </c>
+      <c r="H15" s="47">
+        <v>51151</v>
+      </c>
+      <c r="I15" s="47">
+        <v>42731</v>
+      </c>
+      <c r="J15" s="47">
+        <v>32786</v>
+      </c>
+      <c r="K15" s="47">
+        <v>25905</v>
+      </c>
+      <c r="L15" s="47">
+        <v>25564</v>
+      </c>
+      <c r="M15" s="47">
+        <v>22967</v>
+      </c>
+      <c r="N15" s="47">
+        <v>22261</v>
+      </c>
+      <c r="O15" s="47">
+        <v>22092</v>
+      </c>
+      <c r="P15" s="47">
+        <v>16283</v>
+      </c>
+      <c r="Q15" s="47">
+        <v>10331</v>
+      </c>
+      <c r="R15" s="47">
+        <v>13444</v>
+      </c>
+      <c r="S15" s="47">
+        <f>SUM(C15:R15)</f>
+        <v>437213</v>
+      </c>
       <c r="T15" s="47"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="C16" s="47"/>
+      <c r="A16" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="47">
+        <f t="shared" ref="C16:S16" si="4">SUM(C14:C15)</f>
+        <v>64154</v>
+      </c>
+      <c r="D16" s="47">
+        <f t="shared" si="4"/>
+        <v>52998</v>
+      </c>
+      <c r="E16" s="47">
+        <f t="shared" si="4"/>
+        <v>53030</v>
+      </c>
+      <c r="F16" s="47">
+        <f t="shared" si="4"/>
+        <v>61348</v>
+      </c>
+      <c r="G16" s="47">
+        <f t="shared" si="4"/>
+        <v>70483</v>
+      </c>
+      <c r="H16" s="47">
+        <f t="shared" si="4"/>
+        <v>103292</v>
+      </c>
+      <c r="I16" s="47">
+        <f t="shared" si="4"/>
+        <v>83966</v>
+      </c>
+      <c r="J16" s="47">
+        <f t="shared" si="4"/>
+        <v>62707</v>
+      </c>
+      <c r="K16" s="47">
+        <f t="shared" si="4"/>
+        <v>54068</v>
+      </c>
+      <c r="L16" s="47">
+        <f t="shared" si="4"/>
+        <v>51128</v>
+      </c>
+      <c r="M16" s="47">
+        <f t="shared" si="4"/>
+        <v>48973</v>
+      </c>
+      <c r="N16" s="47">
+        <f t="shared" si="4"/>
+        <v>45912</v>
+      </c>
+      <c r="O16" s="47">
+        <f t="shared" si="4"/>
+        <v>47673</v>
+      </c>
+      <c r="P16" s="47">
+        <f t="shared" si="4"/>
+        <v>35835</v>
+      </c>
+      <c r="Q16" s="47">
+        <f t="shared" si="4"/>
+        <v>24553</v>
+      </c>
+      <c r="R16" s="47">
+        <f t="shared" si="4"/>
+        <v>35757</v>
+      </c>
+      <c r="S16" s="47">
+        <f t="shared" si="4"/>
+        <v>895877</v>
+      </c>
       <c r="T16" s="47"/>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.35">
-      <c r="C17" s="47"/>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A17" s="81"/>
+      <c r="B17" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <f>C16/S16</f>
+        <v>7.161027685720249E-2</v>
+      </c>
+      <c r="D17">
+        <f>D16/S16</f>
+        <v>5.9157674546840691E-2</v>
+      </c>
+      <c r="E17">
+        <f>E16/S16</f>
+        <v>5.9193393735970448E-2</v>
+      </c>
+      <c r="F17">
+        <f>F16/S16</f>
+        <v>6.8478150460386855E-2</v>
+      </c>
+      <c r="G17">
+        <f>G16/S16</f>
+        <v>7.8674862732272394E-2</v>
+      </c>
+      <c r="H17">
+        <f>H16/S16</f>
+        <v>0.11529707761221686</v>
+      </c>
+      <c r="I17">
+        <f>I16/S16</f>
+        <v>9.3724919827163772E-2</v>
+      </c>
+      <c r="J17">
+        <f>J16/S16</f>
+        <v>6.9995099773741257E-2</v>
+      </c>
+      <c r="K17">
+        <f>K16/S16</f>
+        <v>6.0352034933366966E-2</v>
+      </c>
+      <c r="L17">
+        <f>L16/S16</f>
+        <v>5.7070334432070477E-2</v>
+      </c>
+      <c r="M17">
+        <f>M16/S16</f>
+        <v>5.4664870289113349E-2</v>
+      </c>
+      <c r="N17">
+        <f>N16/S16</f>
+        <v>5.1248106603919957E-2</v>
+      </c>
+      <c r="O17">
+        <f>O16/S16</f>
+        <v>5.3213778230716942E-2</v>
+      </c>
+      <c r="P17">
+        <f>P16/S16</f>
+        <v>3.9999910702027172E-2</v>
+      </c>
+      <c r="Q17">
+        <f>Q16/S16</f>
+        <v>2.7406664084466952E-2</v>
+      </c>
+      <c r="R17">
+        <f>R16/S16</f>
+        <v>3.9912845178523393E-2</v>
+      </c>
+      <c r="S17">
+        <f>S16/S16</f>
+        <v>1</v>
+      </c>
       <c r="T17" s="47"/>
       <c r="U17" s="47"/>
       <c r="V17" s="47"/>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C18" s="47"/>
     </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C19" s="47"/>
     </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C20" s="47"/>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C21" s="47"/>
       <c r="S21" s="47"/>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C22" s="47"/>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C23" s="47"/>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C24" s="47"/>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C25" s="47"/>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C26" s="47"/>
     </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C27" s="47"/>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C28" s="47"/>
     </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C29" s="47"/>
     </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C30" s="47"/>
     </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C31" s="47"/>
     </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C32" s="47"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="47"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C34" s="47"/>
     </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C35" s="47"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C36" s="47"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C40" s="47"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C41" s="47"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1981,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2049,7 +2604,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="81" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="34" t="s">
@@ -2108,7 +2663,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="81"/>
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2720,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="34" t="s">
         <v>2</v>
       </c>
@@ -2222,7 +2777,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
@@ -2279,7 +2834,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="70"/>
+      <c r="A6" s="81"/>
       <c r="B6" s="34" t="s">
         <v>4</v>
       </c>
@@ -2336,7 +2891,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="34" t="s">
         <v>5</v>
       </c>
@@ -2393,7 +2948,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="34" t="s">
         <v>6</v>
       </c>
@@ -2450,7 +3005,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="70"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="34" t="s">
         <v>7</v>
       </c>
@@ -2507,7 +3062,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="70"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="34" t="s">
         <v>8</v>
       </c>
@@ -2564,7 +3119,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="70"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="34" t="s">
         <v>9</v>
       </c>
@@ -2621,7 +3176,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="70"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="34" t="s">
         <v>10</v>
       </c>
@@ -2678,7 +3233,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="70"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="34" t="s">
         <v>11</v>
       </c>
@@ -2735,7 +3290,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="70"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="34" t="s">
         <v>12</v>
       </c>
@@ -2792,7 +3347,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="70"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="34" t="s">
         <v>13</v>
       </c>
@@ -2849,7 +3404,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
+      <c r="A16" s="81"/>
       <c r="B16" s="34" t="s">
         <v>14</v>
       </c>
@@ -2906,7 +3461,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="70"/>
+      <c r="A17" s="81"/>
       <c r="B17" s="34" t="s">
         <v>15</v>
       </c>
@@ -2963,7 +3518,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="81" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="48" t="s">
@@ -3022,7 +3577,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="70"/>
+      <c r="A19" s="81"/>
       <c r="B19" s="48" t="s">
         <v>1</v>
       </c>
@@ -3079,7 +3634,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="70"/>
+      <c r="A20" s="81"/>
       <c r="B20" s="48" t="s">
         <v>2</v>
       </c>
@@ -3136,7 +3691,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="70"/>
+      <c r="A21" s="81"/>
       <c r="B21" s="48" t="s">
         <v>3</v>
       </c>
@@ -3193,7 +3748,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="70"/>
+      <c r="A22" s="81"/>
       <c r="B22" s="48" t="s">
         <v>4</v>
       </c>
@@ -3250,7 +3805,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="70"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="48" t="s">
         <v>5</v>
       </c>
@@ -3307,7 +3862,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="70"/>
+      <c r="A24" s="81"/>
       <c r="B24" s="48" t="s">
         <v>6</v>
       </c>
@@ -3364,7 +3919,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="70"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="48" t="s">
         <v>7</v>
       </c>
@@ -3421,7 +3976,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="70"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="48" t="s">
         <v>8</v>
       </c>
@@ -3478,7 +4033,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="70"/>
+      <c r="A27" s="81"/>
       <c r="B27" s="48" t="s">
         <v>9</v>
       </c>
@@ -3535,7 +4090,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
+      <c r="A28" s="81"/>
       <c r="B28" s="48" t="s">
         <v>10</v>
       </c>
@@ -3592,7 +4147,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="70"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="48" t="s">
         <v>11</v>
       </c>
@@ -3649,7 +4204,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="70"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="48" t="s">
         <v>12</v>
       </c>
@@ -3706,7 +4261,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="70"/>
+      <c r="A31" s="81"/>
       <c r="B31" s="48" t="s">
         <v>13</v>
       </c>
@@ -3763,7 +4318,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="70"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="48" t="s">
         <v>14</v>
       </c>
@@ -3820,7 +4375,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A33" s="70"/>
+      <c r="A33" s="81"/>
       <c r="B33" s="48" t="s">
         <v>15</v>
       </c>
@@ -3876,10 +4431,1840 @@
         <v>2.8144326209735691</v>
       </c>
     </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0.61969873863987557</v>
+      </c>
+      <c r="D34">
+        <v>0.51930885326415877</v>
+      </c>
+      <c r="E34">
+        <v>0.27317103093736778</v>
+      </c>
+      <c r="F34">
+        <v>0.1220990843140809</v>
+      </c>
+      <c r="G34">
+        <v>0.17291475806902101</v>
+      </c>
+      <c r="H34">
+        <v>0.31709601117876612</v>
+      </c>
+      <c r="I34">
+        <v>0.5565418204061986</v>
+      </c>
+      <c r="J34">
+        <v>0.56240292718534357</v>
+      </c>
+      <c r="K34">
+        <v>0.21349284282175451</v>
+      </c>
+      <c r="L34">
+        <v>8.079024971058428E-2</v>
+      </c>
+      <c r="M34">
+        <v>6.1796659171411188E-2</v>
+      </c>
+      <c r="N34">
+        <v>2.9986530173469729E-2</v>
+      </c>
+      <c r="O34">
+        <v>2.078519260972914E-2</v>
+      </c>
+      <c r="P34">
+        <v>9.4638499050793794E-3</v>
+      </c>
+      <c r="Q34">
+        <v>2.7711226752344682E-3</v>
+      </c>
+      <c r="R34">
+        <v>4.4855420935287181E-3</v>
+      </c>
+      <c r="S34">
+        <v>3.5668052131556029</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="81"/>
+      <c r="B35" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.31930133357744173</v>
+      </c>
+      <c r="D35">
+        <v>0.98541608337489539</v>
+      </c>
+      <c r="E35">
+        <v>0.4877969736720652</v>
+      </c>
+      <c r="F35">
+        <v>0.16195920244802611</v>
+      </c>
+      <c r="G35">
+        <v>4.3457131507647587E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.19998306063301061</v>
+      </c>
+      <c r="I35">
+        <v>0.51032027296683324</v>
+      </c>
+      <c r="J35">
+        <v>0.645337023249687</v>
+      </c>
+      <c r="K35">
+        <v>0.46191402339646931</v>
+      </c>
+      <c r="L35">
+        <v>0.12776537347105479</v>
+      </c>
+      <c r="M35">
+        <v>5.2259648466374167E-2</v>
+      </c>
+      <c r="N35">
+        <v>2.668950530223094E-2</v>
+      </c>
+      <c r="O35">
+        <v>1.327643914610107E-2</v>
+      </c>
+      <c r="P35">
+        <v>1.020265687875028E-2</v>
+      </c>
+      <c r="Q35">
+        <v>3.9208192751110536E-3</v>
+      </c>
+      <c r="R35">
+        <v>3.3901430134257171E-3</v>
+      </c>
+      <c r="S35">
+        <v>4.0529896903791238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="81"/>
+      <c r="B36" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0.17718134683672379</v>
+      </c>
+      <c r="D36">
+        <v>0.51993231380126026</v>
+      </c>
+      <c r="E36">
+        <v>1.523920062409531</v>
+      </c>
+      <c r="F36">
+        <v>0.40228849022523561</v>
+      </c>
+      <c r="G36">
+        <v>5.9383389650805238E-2</v>
+      </c>
+      <c r="H36">
+        <v>3.9346697096150789E-2</v>
+      </c>
+      <c r="I36">
+        <v>0.19834689605494929</v>
+      </c>
+      <c r="J36">
+        <v>0.48200013919098461</v>
+      </c>
+      <c r="K36">
+        <v>0.55487703325535764</v>
+      </c>
+      <c r="L36">
+        <v>0.21334596097495201</v>
+      </c>
+      <c r="M36">
+        <v>7.9429941595848513E-2</v>
+      </c>
+      <c r="N36">
+        <v>2.4421556195950569E-2</v>
+      </c>
+      <c r="O36">
+        <v>1.256075952087831E-2</v>
+      </c>
+      <c r="P36">
+        <v>1.249583723902436E-2</v>
+      </c>
+      <c r="Q36">
+        <v>8.279824777708342E-3</v>
+      </c>
+      <c r="R36">
+        <v>3.76310749565588E-3</v>
+      </c>
+      <c r="S36">
+        <v>4.3115733563210163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="81"/>
+      <c r="B37" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>8.5270794326373564E-2</v>
+      </c>
+      <c r="D37">
+        <v>0.1634655167866628</v>
+      </c>
+      <c r="E37">
+        <v>0.45802860732744471</v>
+      </c>
+      <c r="F37">
+        <v>1.290056514650987</v>
+      </c>
+      <c r="G37">
+        <v>0.19608956712862941</v>
+      </c>
+      <c r="H37">
+        <v>4.8415237082093387E-2</v>
+      </c>
+      <c r="I37">
+        <v>4.9507148439117819E-2</v>
+      </c>
+      <c r="J37">
+        <v>0.2447208048376496</v>
+      </c>
+      <c r="K37">
+        <v>0.43903350853856721</v>
+      </c>
+      <c r="L37">
+        <v>0.36973979800814699</v>
+      </c>
+      <c r="M37">
+        <v>0.18667622279583851</v>
+      </c>
+      <c r="N37">
+        <v>5.8342071323631568E-2</v>
+      </c>
+      <c r="O37">
+        <v>1.611604249113267E-2</v>
+      </c>
+      <c r="P37">
+        <v>1.5775648331884249E-2</v>
+      </c>
+      <c r="Q37">
+        <v>5.8131818691644936E-3</v>
+      </c>
+      <c r="R37">
+        <v>2.6736776283368159E-3</v>
+      </c>
+      <c r="S37">
+        <v>3.629724341565661</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="81"/>
+      <c r="B38" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>0.1478417185798506</v>
+      </c>
+      <c r="D38">
+        <v>7.0406143057896858E-2</v>
+      </c>
+      <c r="E38">
+        <v>8.4660923615236153E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.35768278848216489</v>
+      </c>
+      <c r="G38">
+        <v>1.208624753028102</v>
+      </c>
+      <c r="H38">
+        <v>0.20884701972396169</v>
+      </c>
+      <c r="I38">
+        <v>5.6970339595179879E-2</v>
+      </c>
+      <c r="J38">
+        <v>2.7083629650777191E-2</v>
+      </c>
+      <c r="K38">
+        <v>0.13670317067111079</v>
+      </c>
+      <c r="L38">
+        <v>0.31934191487618502</v>
+      </c>
+      <c r="M38">
+        <v>0.19062797912647891</v>
+      </c>
+      <c r="N38">
+        <v>0.10800255558228671</v>
+      </c>
+      <c r="O38">
+        <v>1.94651016060754E-2</v>
+      </c>
+      <c r="P38">
+        <v>5.5875465430559974E-3</v>
+      </c>
+      <c r="Q38">
+        <v>4.1289364477471047E-3</v>
+      </c>
+      <c r="R38">
+        <v>3.219008945833397E-3</v>
+      </c>
+      <c r="S38">
+        <v>2.949193529531942</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="81"/>
+      <c r="B39" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>0.3976603189755612</v>
+      </c>
+      <c r="D39">
+        <v>0.17802320481836151</v>
+      </c>
+      <c r="E39">
+        <v>4.3947790376431657E-2</v>
+      </c>
+      <c r="F39">
+        <v>8.290010749152231E-2</v>
+      </c>
+      <c r="G39">
+        <v>0.23194145003234701</v>
+      </c>
+      <c r="H39">
+        <v>0.99295240675387897</v>
+      </c>
+      <c r="I39">
+        <v>0.22154003563811769</v>
+      </c>
+      <c r="J39">
+        <v>3.05630158965145E-2</v>
+      </c>
+      <c r="K39">
+        <v>1.418769497448942E-2</v>
+      </c>
+      <c r="L39">
+        <v>7.0238020714514945E-2</v>
+      </c>
+      <c r="M39">
+        <v>0.1595808418760109</v>
+      </c>
+      <c r="N39">
+        <v>0.1161322460451831</v>
+      </c>
+      <c r="O39">
+        <v>4.3053965173040158E-2</v>
+      </c>
+      <c r="P39">
+        <v>8.0376594078613462E-3</v>
+      </c>
+      <c r="Q39">
+        <v>1.035009265019716E-3</v>
+      </c>
+      <c r="R39">
+        <v>4.1776134695652497E-3</v>
+      </c>
+      <c r="S39">
+        <v>2.5959713809084199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" s="81"/>
+      <c r="B40" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>0.48279883411940788</v>
+      </c>
+      <c r="D40">
+        <v>0.54738936640994307</v>
+      </c>
+      <c r="E40">
+        <v>0.27023775728018817</v>
+      </c>
+      <c r="F40">
+        <v>5.3308474952563301E-2</v>
+      </c>
+      <c r="G40">
+        <v>6.3372805900721585E-2</v>
+      </c>
+      <c r="H40">
+        <v>0.1976240965638193</v>
+      </c>
+      <c r="I40">
+        <v>0.88060706508015019</v>
+      </c>
+      <c r="J40">
+        <v>0.19162270816254409</v>
+      </c>
+      <c r="K40">
+        <v>8.3305812944590107E-2</v>
+      </c>
+      <c r="L40">
+        <v>1.7345128672293451E-2</v>
+      </c>
+      <c r="M40">
+        <v>3.1822033182398263E-2</v>
+      </c>
+      <c r="N40">
+        <v>5.0587499749247047E-2</v>
+      </c>
+      <c r="O40">
+        <v>4.6980189303852747E-2</v>
+      </c>
+      <c r="P40">
+        <v>7.4877167106613962E-3</v>
+      </c>
+      <c r="Q40">
+        <v>3.6112444629112271E-3</v>
+      </c>
+      <c r="R40">
+        <v>2.5532874849723301E-3</v>
+      </c>
+      <c r="S40">
+        <v>2.930654020980263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="81"/>
+      <c r="B41" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>0.45328125058501001</v>
+      </c>
+      <c r="D41">
+        <v>0.74278933093205335</v>
+      </c>
+      <c r="E41">
+        <v>0.60155686875189596</v>
+      </c>
+      <c r="F41">
+        <v>0.23332652289149741</v>
+      </c>
+      <c r="G41">
+        <v>3.001240892200361E-2</v>
+      </c>
+      <c r="H41">
+        <v>3.2099731833460772E-2</v>
+      </c>
+      <c r="I41">
+        <v>0.14567765278742381</v>
+      </c>
+      <c r="J41">
+        <v>0.91703313233725503</v>
+      </c>
+      <c r="K41">
+        <v>0.17685763160578219</v>
+      </c>
+      <c r="L41">
+        <v>3.7459357399074557E-2</v>
+      </c>
+      <c r="M41">
+        <v>2.298654830442929E-2</v>
+      </c>
+      <c r="N41">
+        <v>1.6382851462925129E-2</v>
+      </c>
+      <c r="O41">
+        <v>2.9149293357457778E-2</v>
+      </c>
+      <c r="P41">
+        <v>1.6190687828047751E-2</v>
+      </c>
+      <c r="Q41">
+        <v>6.1502193486830279E-3</v>
+      </c>
+      <c r="R41">
+        <v>1.9332739258649139E-3</v>
+      </c>
+      <c r="S41">
+        <v>3.462886762272865</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" s="81"/>
+      <c r="B42" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>0.2121721018053484</v>
+      </c>
+      <c r="D42">
+        <v>0.50095403332651323</v>
+      </c>
+      <c r="E42">
+        <v>0.65196680337327961</v>
+      </c>
+      <c r="F42">
+        <v>0.44861026055557202</v>
+      </c>
+      <c r="G42">
+        <v>0.1030330929272197</v>
+      </c>
+      <c r="H42">
+        <v>2.6288588418927089E-2</v>
+      </c>
+      <c r="I42">
+        <v>8.9226323910685745E-2</v>
+      </c>
+      <c r="J42">
+        <v>0.18657727677081201</v>
+      </c>
+      <c r="K42">
+        <v>0.73249950590968005</v>
+      </c>
+      <c r="L42">
+        <v>0.1202031506394767</v>
+      </c>
+      <c r="M42">
+        <v>3.6477074419668291E-2</v>
+      </c>
+      <c r="N42">
+        <v>6.6137924499284221E-3</v>
+      </c>
+      <c r="O42">
+        <v>2.3744852860144629E-2</v>
+      </c>
+      <c r="P42">
+        <v>2.532257538368134E-2</v>
+      </c>
+      <c r="Q42">
+        <v>1.1007036058564641E-2</v>
+      </c>
+      <c r="R42">
+        <v>4.9299290451300616E-3</v>
+      </c>
+      <c r="S42">
+        <v>3.1796263978546309</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" s="81"/>
+      <c r="B43" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>0.13625913628933151</v>
+      </c>
+      <c r="D43">
+        <v>0.27871032427025172</v>
+      </c>
+      <c r="E43">
+        <v>0.45379324991841169</v>
+      </c>
+      <c r="F43">
+        <v>0.6183423543320512</v>
+      </c>
+      <c r="G43">
+        <v>0.33837918072304513</v>
+      </c>
+      <c r="H43">
+        <v>8.5128129986149201E-2</v>
+      </c>
+      <c r="I43">
+        <v>3.0915997973674281E-2</v>
+      </c>
+      <c r="J43">
+        <v>9.3554337758299674E-2</v>
+      </c>
+      <c r="K43">
+        <v>0.1652417126260991</v>
+      </c>
+      <c r="L43">
+        <v>0.75766440714440808</v>
+      </c>
+      <c r="M43">
+        <v>0.1429206888384171</v>
+      </c>
+      <c r="N43">
+        <v>3.3595936174832419E-2</v>
+      </c>
+      <c r="O43">
+        <v>1.4120675689961171E-2</v>
+      </c>
+      <c r="P43">
+        <v>9.8963210946687655E-3</v>
+      </c>
+      <c r="Q43">
+        <v>9.1649180869296694E-3</v>
+      </c>
+      <c r="R43">
+        <v>1.458046490213989E-2</v>
+      </c>
+      <c r="S43">
+        <v>3.1822678358086711</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" s="81"/>
+      <c r="B44" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>0.19468034463774619</v>
+      </c>
+      <c r="D44">
+        <v>0.17842525811882259</v>
+      </c>
+      <c r="E44">
+        <v>0.332586995417395</v>
+      </c>
+      <c r="F44">
+        <v>0.41293399957734039</v>
+      </c>
+      <c r="G44">
+        <v>0.35606468712225869</v>
+      </c>
+      <c r="H44">
+        <v>0.22283562066637641</v>
+      </c>
+      <c r="I44">
+        <v>8.839893969807712E-2</v>
+      </c>
+      <c r="J44">
+        <v>5.372579722533382E-2</v>
+      </c>
+      <c r="K44">
+        <v>9.7244756556962603E-2</v>
+      </c>
+      <c r="L44">
+        <v>0.17822478599607389</v>
+      </c>
+      <c r="M44">
+        <v>0.73249236715242605</v>
+      </c>
+      <c r="N44">
+        <v>0.16174567858702751</v>
+      </c>
+      <c r="O44">
+        <v>3.2856463947392438E-2</v>
+      </c>
+      <c r="P44">
+        <v>7.8488109687200359E-3</v>
+      </c>
+      <c r="Q44">
+        <v>8.5607829526352548E-3</v>
+      </c>
+      <c r="R44">
+        <v>1.7963340803741481E-2</v>
+      </c>
+      <c r="S44">
+        <v>3.07658862942833</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="81"/>
+      <c r="B45" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>0.2917246094458063</v>
+      </c>
+      <c r="D45">
+        <v>0.29616139570469119</v>
+      </c>
+      <c r="E45">
+        <v>0.22264573850600691</v>
+      </c>
+      <c r="F45">
+        <v>0.33221013984806957</v>
+      </c>
+      <c r="G45">
+        <v>0.30779020939442508</v>
+      </c>
+      <c r="H45">
+        <v>0.36734582943818639</v>
+      </c>
+      <c r="I45">
+        <v>0.24990875975732291</v>
+      </c>
+      <c r="J45">
+        <v>8.1119869756532514E-2</v>
+      </c>
+      <c r="K45">
+        <v>4.2156613613218347E-2</v>
+      </c>
+      <c r="L45">
+        <v>0.1322265063126363</v>
+      </c>
+      <c r="M45">
+        <v>0.24003017409510971</v>
+      </c>
+      <c r="N45">
+        <v>0.79826001195674778</v>
+      </c>
+      <c r="O45">
+        <v>0.1657354874593196</v>
+      </c>
+      <c r="P45">
+        <v>3.8899001049629088E-2</v>
+      </c>
+      <c r="Q45">
+        <v>6.0501289541545289E-3</v>
+      </c>
+      <c r="R45">
+        <v>1.389074087297909E-2</v>
+      </c>
+      <c r="S45">
+        <v>3.5861552161648351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46" s="81"/>
+      <c r="B46" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>0.31134529409820949</v>
+      </c>
+      <c r="D46">
+        <v>0.28834434669726328</v>
+      </c>
+      <c r="E46">
+        <v>0.2058898648644652</v>
+      </c>
+      <c r="F46">
+        <v>0.18457333798675249</v>
+      </c>
+      <c r="G46">
+        <v>0.13843730865305101</v>
+      </c>
+      <c r="H46">
+        <v>0.19415649132730561</v>
+      </c>
+      <c r="I46">
+        <v>0.24950293862579759</v>
+      </c>
+      <c r="J46">
+        <v>0.17967601058066959</v>
+      </c>
+      <c r="K46">
+        <v>0.1018797966469735</v>
+      </c>
+      <c r="L46">
+        <v>4.8114473019489297E-2</v>
+      </c>
+      <c r="M46">
+        <v>9.8837602955819892E-2</v>
+      </c>
+      <c r="N46">
+        <v>0.20723494786629501</v>
+      </c>
+      <c r="O46">
+        <v>0.66400198425770895</v>
+      </c>
+      <c r="P46">
+        <v>0.1036212259481058</v>
+      </c>
+      <c r="Q46">
+        <v>2.1956604262780909E-2</v>
+      </c>
+      <c r="R46">
+        <v>3.7991763247403202E-3</v>
+      </c>
+      <c r="S46">
+        <v>3.001371404115428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A47" s="81"/>
+      <c r="B47" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>0.21362463702654791</v>
+      </c>
+      <c r="D47">
+        <v>0.32217204248857839</v>
+      </c>
+      <c r="E47">
+        <v>0.29704949340625858</v>
+      </c>
+      <c r="F47">
+        <v>0.18085837972139859</v>
+      </c>
+      <c r="G47">
+        <v>0.1179460963612624</v>
+      </c>
+      <c r="H47">
+        <v>0.1106410184411893</v>
+      </c>
+      <c r="I47">
+        <v>0.1800640744179885</v>
+      </c>
+      <c r="J47">
+        <v>0.24091875751101141</v>
+      </c>
+      <c r="K47">
+        <v>0.25559079997534129</v>
+      </c>
+      <c r="L47">
+        <v>6.7540370646448147E-2</v>
+      </c>
+      <c r="M47">
+        <v>5.9720455420753479E-2</v>
+      </c>
+      <c r="N47">
+        <v>9.0416609239335546E-2</v>
+      </c>
+      <c r="O47">
+        <v>0.14470722386705889</v>
+      </c>
+      <c r="P47">
+        <v>0.60070458771345736</v>
+      </c>
+      <c r="Q47">
+        <v>8.5739884031059102E-2</v>
+      </c>
+      <c r="R47">
+        <v>9.1335633219010153E-3</v>
+      </c>
+      <c r="S47">
+        <v>2.9768279935895898</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48" s="81"/>
+      <c r="B48" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>8.7535051743233033E-2</v>
+      </c>
+      <c r="D48">
+        <v>0.2803146037505162</v>
+      </c>
+      <c r="E48">
+        <v>0.25636190225638023</v>
+      </c>
+      <c r="F48">
+        <v>0.21274286482975721</v>
+      </c>
+      <c r="G48">
+        <v>4.2000323079455573E-2</v>
+      </c>
+      <c r="H48">
+        <v>7.7568571123864852E-2</v>
+      </c>
+      <c r="I48">
+        <v>6.9270788270510475E-2</v>
+      </c>
+      <c r="J48">
+        <v>0.1565752716407488</v>
+      </c>
+      <c r="K48">
+        <v>0.2587905839153285</v>
+      </c>
+      <c r="L48">
+        <v>0.1503111281205069</v>
+      </c>
+      <c r="M48">
+        <v>8.3948871423493762E-2</v>
+      </c>
+      <c r="N48">
+        <v>3.7343648814540963E-2</v>
+      </c>
+      <c r="O48">
+        <v>0.10147899237010211</v>
+      </c>
+      <c r="P48">
+        <v>0.13414629770358341</v>
+      </c>
+      <c r="Q48">
+        <v>0.40151916740089549</v>
+      </c>
+      <c r="R48">
+        <v>9.2435073603816947E-2</v>
+      </c>
+      <c r="S48">
+        <v>2.4423431400467339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49" s="81"/>
+      <c r="B49" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49">
+        <v>0.17867052833943259</v>
+      </c>
+      <c r="D49">
+        <v>0.22723956695633729</v>
+      </c>
+      <c r="E49">
+        <v>0.36993855816546489</v>
+      </c>
+      <c r="F49">
+        <v>0.28608324927924661</v>
+      </c>
+      <c r="G49">
+        <v>7.8801542020079648E-2</v>
+      </c>
+      <c r="H49">
+        <v>6.8464474082245624E-2</v>
+      </c>
+      <c r="I49">
+        <v>8.6063113504558322E-2</v>
+      </c>
+      <c r="J49">
+        <v>0.17261569115783351</v>
+      </c>
+      <c r="K49">
+        <v>0.22253658799590159</v>
+      </c>
+      <c r="L49">
+        <v>0.26296910108123212</v>
+      </c>
+      <c r="M49">
+        <v>0.25285122777986668</v>
+      </c>
+      <c r="N49">
+        <v>8.8713983287576278E-2</v>
+      </c>
+      <c r="O49">
+        <v>3.5285301315390857E-2</v>
+      </c>
+      <c r="P49">
+        <v>6.6994453141113561E-2</v>
+      </c>
+      <c r="Q49">
+        <v>0.1152211397637133</v>
+      </c>
+      <c r="R49">
+        <v>0.3019841031035766</v>
+      </c>
+      <c r="S49">
+        <v>2.8144326209735691</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0.61969873863987557</v>
+      </c>
+      <c r="D50">
+        <v>0.51930885326415877</v>
+      </c>
+      <c r="E50">
+        <v>0.27317103093736778</v>
+      </c>
+      <c r="F50">
+        <v>0.1220990843140809</v>
+      </c>
+      <c r="G50">
+        <v>0.17291475806902101</v>
+      </c>
+      <c r="H50">
+        <v>0.31709601117876612</v>
+      </c>
+      <c r="I50">
+        <v>0.5565418204061986</v>
+      </c>
+      <c r="J50">
+        <v>0.56240292718534357</v>
+      </c>
+      <c r="K50">
+        <v>0.21349284282175451</v>
+      </c>
+      <c r="L50">
+        <v>8.079024971058428E-2</v>
+      </c>
+      <c r="M50">
+        <v>6.1796659171411188E-2</v>
+      </c>
+      <c r="N50">
+        <v>2.9986530173469729E-2</v>
+      </c>
+      <c r="O50">
+        <v>2.078519260972914E-2</v>
+      </c>
+      <c r="P50">
+        <v>9.4638499050793794E-3</v>
+      </c>
+      <c r="Q50">
+        <v>2.7711226752344682E-3</v>
+      </c>
+      <c r="R50">
+        <v>4.4855420935287181E-3</v>
+      </c>
+      <c r="S50">
+        <v>3.5668052131556029</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51" s="81"/>
+      <c r="B51" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0.31930133357744173</v>
+      </c>
+      <c r="D51">
+        <v>0.98541608337489539</v>
+      </c>
+      <c r="E51">
+        <v>0.4877969736720652</v>
+      </c>
+      <c r="F51">
+        <v>0.16195920244802611</v>
+      </c>
+      <c r="G51">
+        <v>4.3457131507647587E-2</v>
+      </c>
+      <c r="H51">
+        <v>0.19998306063301061</v>
+      </c>
+      <c r="I51">
+        <v>0.51032027296683324</v>
+      </c>
+      <c r="J51">
+        <v>0.645337023249687</v>
+      </c>
+      <c r="K51">
+        <v>0.46191402339646931</v>
+      </c>
+      <c r="L51">
+        <v>0.12776537347105479</v>
+      </c>
+      <c r="M51">
+        <v>5.2259648466374167E-2</v>
+      </c>
+      <c r="N51">
+        <v>2.668950530223094E-2</v>
+      </c>
+      <c r="O51">
+        <v>1.327643914610107E-2</v>
+      </c>
+      <c r="P51">
+        <v>1.020265687875028E-2</v>
+      </c>
+      <c r="Q51">
+        <v>3.9208192751110536E-3</v>
+      </c>
+      <c r="R51">
+        <v>3.3901430134257171E-3</v>
+      </c>
+      <c r="S51">
+        <v>4.0529896903791238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A52" s="81"/>
+      <c r="B52" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>0.17718134683672379</v>
+      </c>
+      <c r="D52">
+        <v>0.51993231380126026</v>
+      </c>
+      <c r="E52">
+        <v>1.523920062409531</v>
+      </c>
+      <c r="F52">
+        <v>0.40228849022523561</v>
+      </c>
+      <c r="G52">
+        <v>5.9383389650805238E-2</v>
+      </c>
+      <c r="H52">
+        <v>3.9346697096150789E-2</v>
+      </c>
+      <c r="I52">
+        <v>0.19834689605494929</v>
+      </c>
+      <c r="J52">
+        <v>0.48200013919098461</v>
+      </c>
+      <c r="K52">
+        <v>0.55487703325535764</v>
+      </c>
+      <c r="L52">
+        <v>0.21334596097495201</v>
+      </c>
+      <c r="M52">
+        <v>7.9429941595848513E-2</v>
+      </c>
+      <c r="N52">
+        <v>2.4421556195950569E-2</v>
+      </c>
+      <c r="O52">
+        <v>1.256075952087831E-2</v>
+      </c>
+      <c r="P52">
+        <v>1.249583723902436E-2</v>
+      </c>
+      <c r="Q52">
+        <v>8.279824777708342E-3</v>
+      </c>
+      <c r="R52">
+        <v>3.76310749565588E-3</v>
+      </c>
+      <c r="S52">
+        <v>4.3115733563210163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A53" s="81"/>
+      <c r="B53" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>8.5270794326373564E-2</v>
+      </c>
+      <c r="D53">
+        <v>0.1634655167866628</v>
+      </c>
+      <c r="E53">
+        <v>0.45802860732744471</v>
+      </c>
+      <c r="F53">
+        <v>1.290056514650987</v>
+      </c>
+      <c r="G53">
+        <v>0.19608956712862941</v>
+      </c>
+      <c r="H53">
+        <v>4.8415237082093387E-2</v>
+      </c>
+      <c r="I53">
+        <v>4.9507148439117819E-2</v>
+      </c>
+      <c r="J53">
+        <v>0.2447208048376496</v>
+      </c>
+      <c r="K53">
+        <v>0.43903350853856721</v>
+      </c>
+      <c r="L53">
+        <v>0.36973979800814699</v>
+      </c>
+      <c r="M53">
+        <v>0.18667622279583851</v>
+      </c>
+      <c r="N53">
+        <v>5.8342071323631568E-2</v>
+      </c>
+      <c r="O53">
+        <v>1.611604249113267E-2</v>
+      </c>
+      <c r="P53">
+        <v>1.5775648331884249E-2</v>
+      </c>
+      <c r="Q53">
+        <v>5.8131818691644936E-3</v>
+      </c>
+      <c r="R53">
+        <v>2.6736776283368159E-3</v>
+      </c>
+      <c r="S53">
+        <v>3.629724341565661</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A54" s="81"/>
+      <c r="B54" s="70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>0.1478417185798506</v>
+      </c>
+      <c r="D54">
+        <v>7.0406143057896858E-2</v>
+      </c>
+      <c r="E54">
+        <v>8.4660923615236153E-2</v>
+      </c>
+      <c r="F54">
+        <v>0.35768278848216489</v>
+      </c>
+      <c r="G54">
+        <v>1.208624753028102</v>
+      </c>
+      <c r="H54">
+        <v>0.20884701972396169</v>
+      </c>
+      <c r="I54">
+        <v>5.6970339595179879E-2</v>
+      </c>
+      <c r="J54">
+        <v>2.7083629650777191E-2</v>
+      </c>
+      <c r="K54">
+        <v>0.13670317067111079</v>
+      </c>
+      <c r="L54">
+        <v>0.31934191487618502</v>
+      </c>
+      <c r="M54">
+        <v>0.19062797912647891</v>
+      </c>
+      <c r="N54">
+        <v>0.10800255558228671</v>
+      </c>
+      <c r="O54">
+        <v>1.94651016060754E-2</v>
+      </c>
+      <c r="P54">
+        <v>5.5875465430559974E-3</v>
+      </c>
+      <c r="Q54">
+        <v>4.1289364477471047E-3</v>
+      </c>
+      <c r="R54">
+        <v>3.219008945833397E-3</v>
+      </c>
+      <c r="S54">
+        <v>2.949193529531942</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A55" s="81"/>
+      <c r="B55" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>0.3976603189755612</v>
+      </c>
+      <c r="D55">
+        <v>0.17802320481836151</v>
+      </c>
+      <c r="E55">
+        <v>4.3947790376431657E-2</v>
+      </c>
+      <c r="F55">
+        <v>8.290010749152231E-2</v>
+      </c>
+      <c r="G55">
+        <v>0.23194145003234701</v>
+      </c>
+      <c r="H55">
+        <v>0.99295240675387897</v>
+      </c>
+      <c r="I55">
+        <v>0.22154003563811769</v>
+      </c>
+      <c r="J55">
+        <v>3.05630158965145E-2</v>
+      </c>
+      <c r="K55">
+        <v>1.418769497448942E-2</v>
+      </c>
+      <c r="L55">
+        <v>7.0238020714514945E-2</v>
+      </c>
+      <c r="M55">
+        <v>0.1595808418760109</v>
+      </c>
+      <c r="N55">
+        <v>0.1161322460451831</v>
+      </c>
+      <c r="O55">
+        <v>4.3053965173040158E-2</v>
+      </c>
+      <c r="P55">
+        <v>8.0376594078613462E-3</v>
+      </c>
+      <c r="Q55">
+        <v>1.035009265019716E-3</v>
+      </c>
+      <c r="R55">
+        <v>4.1776134695652497E-3</v>
+      </c>
+      <c r="S55">
+        <v>2.5959713809084199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A56" s="81"/>
+      <c r="B56" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>0.48279883411940788</v>
+      </c>
+      <c r="D56">
+        <v>0.54738936640994307</v>
+      </c>
+      <c r="E56">
+        <v>0.27023775728018817</v>
+      </c>
+      <c r="F56">
+        <v>5.3308474952563301E-2</v>
+      </c>
+      <c r="G56">
+        <v>6.3372805900721585E-2</v>
+      </c>
+      <c r="H56">
+        <v>0.1976240965638193</v>
+      </c>
+      <c r="I56">
+        <v>0.88060706508015019</v>
+      </c>
+      <c r="J56">
+        <v>0.19162270816254409</v>
+      </c>
+      <c r="K56">
+        <v>8.3305812944590107E-2</v>
+      </c>
+      <c r="L56">
+        <v>1.7345128672293451E-2</v>
+      </c>
+      <c r="M56">
+        <v>3.1822033182398263E-2</v>
+      </c>
+      <c r="N56">
+        <v>5.0587499749247047E-2</v>
+      </c>
+      <c r="O56">
+        <v>4.6980189303852747E-2</v>
+      </c>
+      <c r="P56">
+        <v>7.4877167106613962E-3</v>
+      </c>
+      <c r="Q56">
+        <v>3.6112444629112271E-3</v>
+      </c>
+      <c r="R56">
+        <v>2.5532874849723301E-3</v>
+      </c>
+      <c r="S56">
+        <v>2.930654020980263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A57" s="81"/>
+      <c r="B57" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>0.45328125058501001</v>
+      </c>
+      <c r="D57">
+        <v>0.74278933093205335</v>
+      </c>
+      <c r="E57">
+        <v>0.60155686875189596</v>
+      </c>
+      <c r="F57">
+        <v>0.23332652289149741</v>
+      </c>
+      <c r="G57">
+        <v>3.001240892200361E-2</v>
+      </c>
+      <c r="H57">
+        <v>3.2099731833460772E-2</v>
+      </c>
+      <c r="I57">
+        <v>0.14567765278742381</v>
+      </c>
+      <c r="J57">
+        <v>0.91703313233725503</v>
+      </c>
+      <c r="K57">
+        <v>0.17685763160578219</v>
+      </c>
+      <c r="L57">
+        <v>3.7459357399074557E-2</v>
+      </c>
+      <c r="M57">
+        <v>2.298654830442929E-2</v>
+      </c>
+      <c r="N57">
+        <v>1.6382851462925129E-2</v>
+      </c>
+      <c r="O57">
+        <v>2.9149293357457778E-2</v>
+      </c>
+      <c r="P57">
+        <v>1.6190687828047751E-2</v>
+      </c>
+      <c r="Q57">
+        <v>6.1502193486830279E-3</v>
+      </c>
+      <c r="R57">
+        <v>1.9332739258649139E-3</v>
+      </c>
+      <c r="S57">
+        <v>3.462886762272865</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A58" s="81"/>
+      <c r="B58" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>0.2121721018053484</v>
+      </c>
+      <c r="D58">
+        <v>0.50095403332651323</v>
+      </c>
+      <c r="E58">
+        <v>0.65196680337327961</v>
+      </c>
+      <c r="F58">
+        <v>0.44861026055557202</v>
+      </c>
+      <c r="G58">
+        <v>0.1030330929272197</v>
+      </c>
+      <c r="H58">
+        <v>2.6288588418927089E-2</v>
+      </c>
+      <c r="I58">
+        <v>8.9226323910685745E-2</v>
+      </c>
+      <c r="J58">
+        <v>0.18657727677081201</v>
+      </c>
+      <c r="K58">
+        <v>0.73249950590968005</v>
+      </c>
+      <c r="L58">
+        <v>0.1202031506394767</v>
+      </c>
+      <c r="M58">
+        <v>3.6477074419668291E-2</v>
+      </c>
+      <c r="N58">
+        <v>6.6137924499284221E-3</v>
+      </c>
+      <c r="O58">
+        <v>2.3744852860144629E-2</v>
+      </c>
+      <c r="P58">
+        <v>2.532257538368134E-2</v>
+      </c>
+      <c r="Q58">
+        <v>1.1007036058564641E-2</v>
+      </c>
+      <c r="R58">
+        <v>4.9299290451300616E-3</v>
+      </c>
+      <c r="S58">
+        <v>3.1796263978546309</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A59" s="81"/>
+      <c r="B59" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>0.13625913628933151</v>
+      </c>
+      <c r="D59">
+        <v>0.27871032427025172</v>
+      </c>
+      <c r="E59">
+        <v>0.45379324991841169</v>
+      </c>
+      <c r="F59">
+        <v>0.6183423543320512</v>
+      </c>
+      <c r="G59">
+        <v>0.33837918072304513</v>
+      </c>
+      <c r="H59">
+        <v>8.5128129986149201E-2</v>
+      </c>
+      <c r="I59">
+        <v>3.0915997973674281E-2</v>
+      </c>
+      <c r="J59">
+        <v>9.3554337758299674E-2</v>
+      </c>
+      <c r="K59">
+        <v>0.1652417126260991</v>
+      </c>
+      <c r="L59">
+        <v>0.75766440714440808</v>
+      </c>
+      <c r="M59">
+        <v>0.1429206888384171</v>
+      </c>
+      <c r="N59">
+        <v>3.3595936174832419E-2</v>
+      </c>
+      <c r="O59">
+        <v>1.4120675689961171E-2</v>
+      </c>
+      <c r="P59">
+        <v>9.8963210946687655E-3</v>
+      </c>
+      <c r="Q59">
+        <v>9.1649180869296694E-3</v>
+      </c>
+      <c r="R59">
+        <v>1.458046490213989E-2</v>
+      </c>
+      <c r="S59">
+        <v>3.1822678358086711</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A60" s="81"/>
+      <c r="B60" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>0.19468034463774619</v>
+      </c>
+      <c r="D60">
+        <v>0.17842525811882259</v>
+      </c>
+      <c r="E60">
+        <v>0.332586995417395</v>
+      </c>
+      <c r="F60">
+        <v>0.41293399957734039</v>
+      </c>
+      <c r="G60">
+        <v>0.35606468712225869</v>
+      </c>
+      <c r="H60">
+        <v>0.22283562066637641</v>
+      </c>
+      <c r="I60">
+        <v>8.839893969807712E-2</v>
+      </c>
+      <c r="J60">
+        <v>5.372579722533382E-2</v>
+      </c>
+      <c r="K60">
+        <v>9.7244756556962603E-2</v>
+      </c>
+      <c r="L60">
+        <v>0.17822478599607389</v>
+      </c>
+      <c r="M60">
+        <v>0.73249236715242605</v>
+      </c>
+      <c r="N60">
+        <v>0.16174567858702751</v>
+      </c>
+      <c r="O60">
+        <v>3.2856463947392438E-2</v>
+      </c>
+      <c r="P60">
+        <v>7.8488109687200359E-3</v>
+      </c>
+      <c r="Q60">
+        <v>8.5607829526352548E-3</v>
+      </c>
+      <c r="R60">
+        <v>1.7963340803741481E-2</v>
+      </c>
+      <c r="S60">
+        <v>3.07658862942833</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A61" s="81"/>
+      <c r="B61" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>0.2917246094458063</v>
+      </c>
+      <c r="D61">
+        <v>0.29616139570469119</v>
+      </c>
+      <c r="E61">
+        <v>0.22264573850600691</v>
+      </c>
+      <c r="F61">
+        <v>0.33221013984806957</v>
+      </c>
+      <c r="G61">
+        <v>0.30779020939442508</v>
+      </c>
+      <c r="H61">
+        <v>0.36734582943818639</v>
+      </c>
+      <c r="I61">
+        <v>0.24990875975732291</v>
+      </c>
+      <c r="J61">
+        <v>8.1119869756532514E-2</v>
+      </c>
+      <c r="K61">
+        <v>4.2156613613218347E-2</v>
+      </c>
+      <c r="L61">
+        <v>0.1322265063126363</v>
+      </c>
+      <c r="M61">
+        <v>0.24003017409510971</v>
+      </c>
+      <c r="N61">
+        <v>0.79826001195674778</v>
+      </c>
+      <c r="O61">
+        <v>0.1657354874593196</v>
+      </c>
+      <c r="P61">
+        <v>3.8899001049629088E-2</v>
+      </c>
+      <c r="Q61">
+        <v>6.0501289541545289E-3</v>
+      </c>
+      <c r="R61">
+        <v>1.389074087297909E-2</v>
+      </c>
+      <c r="S61">
+        <v>3.5861552161648351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A62" s="81"/>
+      <c r="B62" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>0.31134529409820949</v>
+      </c>
+      <c r="D62">
+        <v>0.28834434669726328</v>
+      </c>
+      <c r="E62">
+        <v>0.2058898648644652</v>
+      </c>
+      <c r="F62">
+        <v>0.18457333798675249</v>
+      </c>
+      <c r="G62">
+        <v>0.13843730865305101</v>
+      </c>
+      <c r="H62">
+        <v>0.19415649132730561</v>
+      </c>
+      <c r="I62">
+        <v>0.24950293862579759</v>
+      </c>
+      <c r="J62">
+        <v>0.17967601058066959</v>
+      </c>
+      <c r="K62">
+        <v>0.1018797966469735</v>
+      </c>
+      <c r="L62">
+        <v>4.8114473019489297E-2</v>
+      </c>
+      <c r="M62">
+        <v>9.8837602955819892E-2</v>
+      </c>
+      <c r="N62">
+        <v>0.20723494786629501</v>
+      </c>
+      <c r="O62">
+        <v>0.66400198425770895</v>
+      </c>
+      <c r="P62">
+        <v>0.1036212259481058</v>
+      </c>
+      <c r="Q62">
+        <v>2.1956604262780909E-2</v>
+      </c>
+      <c r="R62">
+        <v>3.7991763247403202E-3</v>
+      </c>
+      <c r="S62">
+        <v>3.001371404115428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A63" s="81"/>
+      <c r="B63" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <v>0.21362463702654791</v>
+      </c>
+      <c r="D63">
+        <v>0.32217204248857839</v>
+      </c>
+      <c r="E63">
+        <v>0.29704949340625858</v>
+      </c>
+      <c r="F63">
+        <v>0.18085837972139859</v>
+      </c>
+      <c r="G63">
+        <v>0.1179460963612624</v>
+      </c>
+      <c r="H63">
+        <v>0.1106410184411893</v>
+      </c>
+      <c r="I63">
+        <v>0.1800640744179885</v>
+      </c>
+      <c r="J63">
+        <v>0.24091875751101141</v>
+      </c>
+      <c r="K63">
+        <v>0.25559079997534129</v>
+      </c>
+      <c r="L63">
+        <v>6.7540370646448147E-2</v>
+      </c>
+      <c r="M63">
+        <v>5.9720455420753479E-2</v>
+      </c>
+      <c r="N63">
+        <v>9.0416609239335546E-2</v>
+      </c>
+      <c r="O63">
+        <v>0.14470722386705889</v>
+      </c>
+      <c r="P63">
+        <v>0.60070458771345736</v>
+      </c>
+      <c r="Q63">
+        <v>8.5739884031059102E-2</v>
+      </c>
+      <c r="R63">
+        <v>9.1335633219010153E-3</v>
+      </c>
+      <c r="S63">
+        <v>2.9768279935895898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A64" s="81"/>
+      <c r="B64" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <v>8.7535051743233033E-2</v>
+      </c>
+      <c r="D64">
+        <v>0.2803146037505162</v>
+      </c>
+      <c r="E64">
+        <v>0.25636190225638023</v>
+      </c>
+      <c r="F64">
+        <v>0.21274286482975721</v>
+      </c>
+      <c r="G64">
+        <v>4.2000323079455573E-2</v>
+      </c>
+      <c r="H64">
+        <v>7.7568571123864852E-2</v>
+      </c>
+      <c r="I64">
+        <v>6.9270788270510475E-2</v>
+      </c>
+      <c r="J64">
+        <v>0.1565752716407488</v>
+      </c>
+      <c r="K64">
+        <v>0.2587905839153285</v>
+      </c>
+      <c r="L64">
+        <v>0.1503111281205069</v>
+      </c>
+      <c r="M64">
+        <v>8.3948871423493762E-2</v>
+      </c>
+      <c r="N64">
+        <v>3.7343648814540963E-2</v>
+      </c>
+      <c r="O64">
+        <v>0.10147899237010211</v>
+      </c>
+      <c r="P64">
+        <v>0.13414629770358341</v>
+      </c>
+      <c r="Q64">
+        <v>0.40151916740089549</v>
+      </c>
+      <c r="R64">
+        <v>9.2435073603816947E-2</v>
+      </c>
+      <c r="S64">
+        <v>2.4423431400467339</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A65" s="81"/>
+      <c r="B65" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65">
+        <v>0.17867052833943259</v>
+      </c>
+      <c r="D65">
+        <v>0.22723956695633729</v>
+      </c>
+      <c r="E65">
+        <v>0.36993855816546489</v>
+      </c>
+      <c r="F65">
+        <v>0.28608324927924661</v>
+      </c>
+      <c r="G65">
+        <v>7.8801542020079648E-2</v>
+      </c>
+      <c r="H65">
+        <v>6.8464474082245624E-2</v>
+      </c>
+      <c r="I65">
+        <v>8.6063113504558322E-2</v>
+      </c>
+      <c r="J65">
+        <v>0.17261569115783351</v>
+      </c>
+      <c r="K65">
+        <v>0.22253658799590159</v>
+      </c>
+      <c r="L65">
+        <v>0.26296910108123212</v>
+      </c>
+      <c r="M65">
+        <v>0.25285122777986668</v>
+      </c>
+      <c r="N65">
+        <v>8.8713983287576278E-2</v>
+      </c>
+      <c r="O65">
+        <v>3.5285301315390857E-2</v>
+      </c>
+      <c r="P65">
+        <v>6.6994453141113561E-2</v>
+      </c>
+      <c r="Q65">
+        <v>0.1152211397637133</v>
+      </c>
+      <c r="R65">
+        <v>0.3019841031035766</v>
+      </c>
+      <c r="S65">
+        <v>2.8144326209735691</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="A18:A33"/>
+    <mergeCell ref="A34:A49"/>
+    <mergeCell ref="A50:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3890,7 +6275,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3963,7 +6348,7 @@
         <v>4.3999999999999995</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:G3" si="0">13.2/3</f>
+        <f t="shared" ref="F3:G5" si="0">13.2/3</f>
         <v>4.3999999999999995</v>
       </c>
       <c r="G3">
@@ -3972,10 +6357,56 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="49"/>
+      <c r="A4" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="50">
+        <v>47.4</v>
+      </c>
+      <c r="C4">
+        <v>25.9</v>
+      </c>
+      <c r="D4">
+        <v>12.6</v>
+      </c>
+      <c r="E4">
+        <f>14.1/3</f>
+        <v>4.7</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:G4" si="1">14.1/3</f>
+        <v>4.7</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="49"/>
+      <c r="A5" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="50">
+        <v>35.5</v>
+      </c>
+      <c r="C5">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="D5">
+        <v>13.5</v>
+      </c>
+      <c r="E5">
+        <f>16.3/3</f>
+        <v>5.4333333333333336</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:G5" si="2">16.3/3</f>
+        <v>5.4333333333333336</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>5.4333333333333336</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="49"/>
@@ -3987,10 +6418,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4103,6 +6534,70 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>110</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>110</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4111,10 +6606,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52C3A41-4386-8748-9118-AB71B95DC696}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4226,6 +6721,70 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="16">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
+        <v>110</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="16">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>110</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="17">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4233,10 +6792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE614D0C-9307-C648-846E-6D3BD3F68B91}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4349,6 +6908,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="9">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="35">
+        <v>1</v>
+      </c>
+      <c r="F4" s="35">
+        <v>5</v>
+      </c>
+      <c r="G4" s="35">
+        <v>18</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="9">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="35">
+        <v>1</v>
+      </c>
+      <c r="F5" s="35">
+        <v>5</v>
+      </c>
+      <c r="G5" s="35">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4356,10 +6979,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34677627-FE5B-AA47-B68E-F56E9F3F7CD6}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4471,6 +7094,70 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="16">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>18</v>
+      </c>
+      <c r="G4" s="12">
+        <v>65</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="16">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12">
+        <v>65</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="17">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4478,10 +7165,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642FC35E-47F5-4C37-873D-2E19575CE65D}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4498,7 +7185,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="75" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="24" t="s">
@@ -4527,54 +7214,104 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="72" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="79">
+      <c r="E2" s="73">
         <v>0</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="73" t="s">
         <v>95</v>
       </c>
       <c r="H2" s="20"/>
-      <c r="I2" s="78"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="77" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="84">
+      <c r="E3" s="78">
         <v>0</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="86"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="73">
+        <v>0</v>
+      </c>
+      <c r="F4" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="72"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="78" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="78">
+        <v>0</v>
+      </c>
+      <c r="F5" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="78" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="79"/>
+      <c r="I5" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4584,10 +7321,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4653,7 +7390,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="82" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -4694,7 +7431,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="72"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="36" t="s">
         <v>71</v>
       </c>
@@ -4733,7 +7470,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="72"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="36" t="s">
         <v>72</v>
       </c>
@@ -4741,7 +7478,7 @@
         <v>76</v>
       </c>
       <c r="D4" s="38">
-        <v>0.218</v>
+        <v>0.15</v>
       </c>
       <c r="E4" s="42">
         <v>1</v>
@@ -4772,7 +7509,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="72"/>
+      <c r="A5" s="83"/>
       <c r="B5" s="36" t="s">
         <v>73</v>
       </c>
@@ -4780,7 +7517,7 @@
         <v>83</v>
       </c>
       <c r="D5" s="38">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="E5" s="42">
         <v>1</v>
@@ -4811,7 +7548,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="72"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="36" t="s">
         <v>74</v>
       </c>
@@ -4819,7 +7556,7 @@
         <v>84</v>
       </c>
       <c r="D6" s="38">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="E6" s="37">
         <v>1</v>
@@ -4847,7 +7584,7 @@
       <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="72"/>
+      <c r="A7" s="83"/>
       <c r="B7" s="36" t="s">
         <v>77</v>
       </c>
@@ -4881,7 +7618,7 @@
       <c r="N7" s="39"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="72"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="36" t="s">
         <v>79</v>
       </c>
@@ -4889,7 +7626,7 @@
         <v>65</v>
       </c>
       <c r="D8" s="38">
-        <v>0.55000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="E8" s="42">
         <v>1</v>
@@ -4915,7 +7652,7 @@
       <c r="N8" s="46"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="73"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="27" t="s">
         <v>75</v>
       </c>
@@ -4923,7 +7660,7 @@
         <v>65</v>
       </c>
       <c r="D9" s="33">
-        <v>0.45</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E9" s="41">
         <v>1</v>
@@ -4949,7 +7686,7 @@
       <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="85" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="51" t="s">
@@ -4990,7 +7727,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="75"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="57" t="s">
         <v>71</v>
       </c>
@@ -5029,7 +7766,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="75"/>
+      <c r="A12" s="86"/>
       <c r="B12" s="57" t="s">
         <v>72</v>
       </c>
@@ -5037,7 +7774,7 @@
         <v>76</v>
       </c>
       <c r="D12" s="58">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="61">
         <v>1</v>
@@ -5068,7 +7805,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="75"/>
+      <c r="A13" s="86"/>
       <c r="B13" s="57" t="s">
         <v>73</v>
       </c>
@@ -5076,7 +7813,7 @@
         <v>83</v>
       </c>
       <c r="D13" s="58">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="E13" s="61">
         <v>1</v>
@@ -5107,7 +7844,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="75"/>
+      <c r="A14" s="86"/>
       <c r="B14" s="57" t="s">
         <v>74</v>
       </c>
@@ -5143,7 +7880,7 @@
       <c r="N14" s="59"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="75"/>
+      <c r="A15" s="86"/>
       <c r="B15" s="57" t="s">
         <v>77</v>
       </c>
@@ -5177,7 +7914,7 @@
       <c r="N15" s="59"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="75"/>
+      <c r="A16" s="86"/>
       <c r="B16" s="57" t="s">
         <v>79</v>
       </c>
@@ -5211,7 +7948,7 @@
       <c r="N16" s="62"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="76"/>
+      <c r="A17" s="87"/>
       <c r="B17" s="63" t="s">
         <v>75</v>
       </c>
@@ -5244,10 +7981,604 @@
       <c r="M17" s="69"/>
       <c r="N17" s="68"/>
     </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
+      <c r="H18" s="19">
+        <v>1</v>
+      </c>
+      <c r="I18" s="19">
+        <v>1</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20">
+        <v>43900</v>
+      </c>
+      <c r="N18" s="45">
+        <f>M19</f>
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="83"/>
+      <c r="B19" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="37">
+        <v>1</v>
+      </c>
+      <c r="F19" s="37">
+        <v>1</v>
+      </c>
+      <c r="G19" s="37">
+        <v>1</v>
+      </c>
+      <c r="H19" s="37">
+        <v>1</v>
+      </c>
+      <c r="I19" s="37">
+        <v>1</v>
+      </c>
+      <c r="J19" s="37">
+        <v>0</v>
+      </c>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="39">
+        <v>43905</v>
+      </c>
+      <c r="N19" s="45">
+        <f t="shared" ref="N19:N21" si="0">M20</f>
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="83"/>
+      <c r="B20" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="38">
+        <v>0.218</v>
+      </c>
+      <c r="E20" s="42">
+        <v>1</v>
+      </c>
+      <c r="F20" s="37">
+        <v>1</v>
+      </c>
+      <c r="G20" s="37">
+        <v>1</v>
+      </c>
+      <c r="H20" s="37">
+        <v>1</v>
+      </c>
+      <c r="I20" s="37">
+        <v>1</v>
+      </c>
+      <c r="J20" s="37">
+        <v>0</v>
+      </c>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="39">
+        <v>43912</v>
+      </c>
+      <c r="N20" s="45">
+        <f t="shared" si="0"/>
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="83"/>
+      <c r="B21" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="38">
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="42">
+        <v>1</v>
+      </c>
+      <c r="F21" s="37">
+        <v>1</v>
+      </c>
+      <c r="G21" s="37">
+        <v>1</v>
+      </c>
+      <c r="H21" s="37">
+        <v>1</v>
+      </c>
+      <c r="I21" s="37">
+        <v>1</v>
+      </c>
+      <c r="J21" s="37">
+        <v>0</v>
+      </c>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="39">
+        <v>43952</v>
+      </c>
+      <c r="N21" s="45">
+        <f t="shared" si="0"/>
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="83"/>
+      <c r="B22" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="37">
+        <v>1</v>
+      </c>
+      <c r="F22" s="37">
+        <v>1</v>
+      </c>
+      <c r="G22" s="37">
+        <v>1</v>
+      </c>
+      <c r="H22" s="37">
+        <v>1</v>
+      </c>
+      <c r="I22" s="37">
+        <v>1</v>
+      </c>
+      <c r="J22" s="37">
+        <v>0</v>
+      </c>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="39">
+        <v>43977</v>
+      </c>
+      <c r="N22" s="39"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="83"/>
+      <c r="B23" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="37">
+        <v>1</v>
+      </c>
+      <c r="F23" s="37">
+        <v>1</v>
+      </c>
+      <c r="G23" s="37">
+        <v>1</v>
+      </c>
+      <c r="H23" s="37">
+        <v>1</v>
+      </c>
+      <c r="I23" s="37">
+        <v>1</v>
+      </c>
+      <c r="J23" s="37">
+        <v>0</v>
+      </c>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="83"/>
+      <c r="B24" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="38">
+        <v>0.38</v>
+      </c>
+      <c r="E24" s="42">
+        <v>1</v>
+      </c>
+      <c r="F24" s="37">
+        <v>1</v>
+      </c>
+      <c r="G24" s="37">
+        <v>1</v>
+      </c>
+      <c r="H24" s="37">
+        <v>1</v>
+      </c>
+      <c r="I24" s="37">
+        <v>1</v>
+      </c>
+      <c r="J24" s="37">
+        <v>0</v>
+      </c>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="46"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="84"/>
+      <c r="B25" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0.35</v>
+      </c>
+      <c r="E25" s="41">
+        <v>1</v>
+      </c>
+      <c r="F25" s="21">
+        <v>1</v>
+      </c>
+      <c r="G25" s="21">
+        <v>1</v>
+      </c>
+      <c r="H25" s="21">
+        <v>1</v>
+      </c>
+      <c r="I25" s="21">
+        <v>1</v>
+      </c>
+      <c r="J25" s="21">
+        <v>0</v>
+      </c>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="22"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="53">
+        <v>0.9</v>
+      </c>
+      <c r="E26" s="54">
+        <v>1</v>
+      </c>
+      <c r="F26" s="54">
+        <v>1</v>
+      </c>
+      <c r="G26" s="54">
+        <v>1</v>
+      </c>
+      <c r="H26" s="54">
+        <v>1</v>
+      </c>
+      <c r="I26" s="54">
+        <v>1</v>
+      </c>
+      <c r="J26" s="54">
+        <v>0</v>
+      </c>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="55">
+        <v>43900</v>
+      </c>
+      <c r="N26" s="56">
+        <f>M27</f>
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="86"/>
+      <c r="B27" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="58">
+        <v>0.6</v>
+      </c>
+      <c r="E27" s="35">
+        <v>1</v>
+      </c>
+      <c r="F27" s="35">
+        <v>1</v>
+      </c>
+      <c r="G27" s="35">
+        <v>1</v>
+      </c>
+      <c r="H27" s="35">
+        <v>1</v>
+      </c>
+      <c r="I27" s="35">
+        <v>1</v>
+      </c>
+      <c r="J27" s="35">
+        <v>0</v>
+      </c>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="59">
+        <v>43905</v>
+      </c>
+      <c r="N27" s="56">
+        <f t="shared" ref="N27:N29" si="1">M28</f>
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="86"/>
+      <c r="B28" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="58">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="61">
+        <v>1</v>
+      </c>
+      <c r="F28" s="35">
+        <v>1</v>
+      </c>
+      <c r="G28" s="35">
+        <v>1</v>
+      </c>
+      <c r="H28" s="35">
+        <v>1</v>
+      </c>
+      <c r="I28" s="35">
+        <v>1</v>
+      </c>
+      <c r="J28" s="35">
+        <v>0</v>
+      </c>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="59">
+        <v>43912</v>
+      </c>
+      <c r="N28" s="56">
+        <f t="shared" si="1"/>
+        <v>43952</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="86"/>
+      <c r="B29" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="58">
+        <v>0.22</v>
+      </c>
+      <c r="E29" s="61">
+        <v>1</v>
+      </c>
+      <c r="F29" s="35">
+        <v>1</v>
+      </c>
+      <c r="G29" s="35">
+        <v>1</v>
+      </c>
+      <c r="H29" s="35">
+        <v>1</v>
+      </c>
+      <c r="I29" s="35">
+        <v>1</v>
+      </c>
+      <c r="J29" s="35">
+        <v>0</v>
+      </c>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="59">
+        <v>43952</v>
+      </c>
+      <c r="N29" s="56">
+        <f t="shared" si="1"/>
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="86"/>
+      <c r="B30" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="58">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E30" s="35">
+        <v>1</v>
+      </c>
+      <c r="F30" s="35">
+        <v>1</v>
+      </c>
+      <c r="G30" s="35">
+        <v>1</v>
+      </c>
+      <c r="H30" s="35">
+        <v>1</v>
+      </c>
+      <c r="I30" s="35">
+        <v>1</v>
+      </c>
+      <c r="J30" s="35">
+        <v>0</v>
+      </c>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="59">
+        <v>43977</v>
+      </c>
+      <c r="N30" s="59"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="86"/>
+      <c r="B31" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="58">
+        <v>0.3</v>
+      </c>
+      <c r="E31" s="35">
+        <v>1</v>
+      </c>
+      <c r="F31" s="35">
+        <v>1</v>
+      </c>
+      <c r="G31" s="35">
+        <v>1</v>
+      </c>
+      <c r="H31" s="35">
+        <v>1</v>
+      </c>
+      <c r="I31" s="35">
+        <v>1</v>
+      </c>
+      <c r="J31" s="35">
+        <v>0</v>
+      </c>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="86"/>
+      <c r="B32" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="58">
+        <v>0.32</v>
+      </c>
+      <c r="E32" s="61">
+        <v>1</v>
+      </c>
+      <c r="F32" s="35">
+        <v>1</v>
+      </c>
+      <c r="G32" s="35">
+        <v>1</v>
+      </c>
+      <c r="H32" s="35">
+        <v>1</v>
+      </c>
+      <c r="I32" s="35">
+        <v>1</v>
+      </c>
+      <c r="J32" s="35">
+        <v>0</v>
+      </c>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="62"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A33" s="87"/>
+      <c r="B33" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="65">
+        <v>0.3</v>
+      </c>
+      <c r="E33" s="66">
+        <v>1</v>
+      </c>
+      <c r="F33" s="67">
+        <v>1</v>
+      </c>
+      <c r="G33" s="67">
+        <v>1</v>
+      </c>
+      <c r="H33" s="67">
+        <v>1</v>
+      </c>
+      <c r="I33" s="67">
+        <v>1</v>
+      </c>
+      <c r="J33" s="67">
+        <v>0</v>
+      </c>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A33"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5257,10 +8588,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5392,7 +8723,7 @@
         <v>50</v>
       </c>
       <c r="P2">
-        <v>60</v>
+        <v>173</v>
       </c>
       <c r="Q2">
         <v>1000</v>
@@ -5401,7 +8732,7 @@
         <v>1000</v>
       </c>
       <c r="S2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="T2">
         <v>1</v>
@@ -5474,7 +8805,7 @@
         <v>1000</v>
       </c>
       <c r="S3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="T3">
         <v>1</v>
@@ -5486,6 +8817,152 @@
         <v>3</v>
       </c>
       <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43886</v>
+      </c>
+      <c r="C4" s="2">
+        <f>B4+400</f>
+        <v>44286</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+      <c r="F4">
+        <f>age_sex!S12/other_par!E4</f>
+        <v>3.8378100000000002</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4">
+        <v>1.2</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L4">
+        <v>0.3</v>
+      </c>
+      <c r="M4">
+        <v>0.1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>50</v>
+      </c>
+      <c r="P4">
+        <v>173</v>
+      </c>
+      <c r="Q4">
+        <v>200</v>
+      </c>
+      <c r="R4">
+        <v>1000</v>
+      </c>
+      <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0.7</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43886</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5+400</f>
+        <v>44286</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+      <c r="F5">
+        <f>age_sex!S16/other_par!E5</f>
+        <v>8.9587699999999995</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>1.2</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+      <c r="M5">
+        <v>0.1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>50</v>
+      </c>
+      <c r="P5">
+        <v>173</v>
+      </c>
+      <c r="Q5">
+        <v>1000</v>
+      </c>
+      <c r="R5">
+        <v>1000</v>
+      </c>
+      <c r="S5">
+        <v>40</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0.7</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Boston Cleveland and Columbus updates
</commit_message>
<xml_diff>
--- a/data/input_data_US_Boston.xlsx
+++ b/data/input_data_US_Boston.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anna.palmer\Documents\GitHub\covasim-australia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF18292-9D52-44F7-8B35-B45F92A646CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C3C3DE-3820-47EA-A3B3-6193FC0D2E31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14610" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="839" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age_sex" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,12 @@
     <sheet name="other_par" sheetId="6" r:id="rId9"/>
     <sheet name="contact matrices-home" sheetId="7" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,18 +45,36 @@
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{B1C3BEE0-D7D8-4E76-BD65-AA803FFBCB0D}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The time to trace contacts, applied to all targeted layers for this policy</t>
+        </r>
       </text>
     </comment>
     <comment ref="G1" authorId="1" shapeId="0" xr:uid="{0749A4AD-0048-4C3C-B625-BFE1D64E5CF7}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The days on which the coverage changes</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -73,10 +89,19 @@
   <commentList>
     <comment ref="R1" authorId="0" shapeId="0" xr:uid="{7833F806-E614-7449-968E-2A674530B08E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Only used if the the new_tests column of the epi data is incorrectly specified</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1298,13 +1323,13 @@
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1363,7 +1388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
         <v>80</v>
       </c>
@@ -1423,7 +1448,7 @@
         <v>352654</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="81"/>
       <c r="B3" s="1" t="s">
         <v>20</v>
@@ -1481,7 +1506,7 @@
         <v>326759</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="81" t="s">
         <v>80</v>
       </c>
@@ -1557,7 +1582,7 @@
         <v>679413</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="81"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -1631,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="81" t="s">
         <v>85</v>
       </c>
@@ -1691,7 +1716,7 @@
         <v>112660</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="81"/>
       <c r="B7" s="48" t="s">
         <v>20</v>
@@ -1749,7 +1774,7 @@
         <v>96634</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="81" t="s">
         <v>85</v>
       </c>
@@ -1825,7 +1850,7 @@
         <v>209294</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="81"/>
       <c r="B9" s="48" t="s">
         <v>21</v>
@@ -1899,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="81" t="s">
         <v>99</v>
       </c>
@@ -1959,7 +1984,7 @@
         <v>195300</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="81"/>
       <c r="B11" s="70" t="s">
         <v>20</v>
@@ -2017,7 +2042,7 @@
         <v>188481</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="81" t="s">
         <v>99</v>
       </c>
@@ -2093,7 +2118,7 @@
         <v>383781</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="81"/>
       <c r="B13" s="70" t="s">
         <v>21</v>
@@ -2167,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="81" t="s">
         <v>100</v>
       </c>
@@ -2229,7 +2254,7 @@
       <c r="U14" s="47"/>
       <c r="V14" s="47"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="81"/>
       <c r="B15" s="70" t="s">
         <v>20</v>
@@ -2288,7 +2313,7 @@
       </c>
       <c r="T15" s="47"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="81" t="s">
         <v>100</v>
       </c>
@@ -2365,7 +2390,7 @@
       </c>
       <c r="T16" s="47"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="81"/>
       <c r="B17" s="70" t="s">
         <v>21</v>
@@ -2442,81 +2467,81 @@
       <c r="U17" s="47"/>
       <c r="V17" s="47"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C18" s="47"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C19" s="47"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C20" s="47"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C21" s="47"/>
       <c r="S21" s="47"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C22" s="47"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C23" s="47"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C24" s="47"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C25" s="47"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C26" s="47"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C27" s="47"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C28" s="47"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C29" s="47"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C30" s="47"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C31" s="47"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C32" s="47"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="47"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="47"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="47"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C36" s="47"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="47"/>
       <c r="D37" s="47"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="47"/>
       <c r="D38" s="47"/>
       <c r="E38" s="47"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="47"/>
       <c r="D39" s="47"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="47"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="47"/>
     </row>
   </sheetData>
@@ -2542,9 +2567,9 @@
       <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2603,7 +2628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
         <v>80</v>
       </c>
@@ -2662,7 +2687,7 @@
         <v>3.5668052131556029</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="81"/>
       <c r="B3" s="34" t="s">
         <v>1</v>
@@ -2719,7 +2744,7 @@
         <v>4.0529896903791238</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="81"/>
       <c r="B4" s="34" t="s">
         <v>2</v>
@@ -2776,7 +2801,7 @@
         <v>4.3115733563210163</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="81"/>
       <c r="B5" s="34" t="s">
         <v>3</v>
@@ -2833,7 +2858,7 @@
         <v>3.629724341565661</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="81"/>
       <c r="B6" s="34" t="s">
         <v>4</v>
@@ -2890,7 +2915,7 @@
         <v>2.949193529531942</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="81"/>
       <c r="B7" s="34" t="s">
         <v>5</v>
@@ -2947,7 +2972,7 @@
         <v>2.5959713809084199</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="81"/>
       <c r="B8" s="34" t="s">
         <v>6</v>
@@ -3004,7 +3029,7 @@
         <v>2.930654020980263</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="81"/>
       <c r="B9" s="34" t="s">
         <v>7</v>
@@ -3061,7 +3086,7 @@
         <v>3.462886762272865</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="81"/>
       <c r="B10" s="34" t="s">
         <v>8</v>
@@ -3118,7 +3143,7 @@
         <v>3.1796263978546309</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="81"/>
       <c r="B11" s="34" t="s">
         <v>9</v>
@@ -3175,7 +3200,7 @@
         <v>3.1822678358086711</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="81"/>
       <c r="B12" s="34" t="s">
         <v>10</v>
@@ -3232,7 +3257,7 @@
         <v>3.07658862942833</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="81"/>
       <c r="B13" s="34" t="s">
         <v>11</v>
@@ -3289,7 +3314,7 @@
         <v>3.5861552161648351</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="81"/>
       <c r="B14" s="34" t="s">
         <v>12</v>
@@ -3346,7 +3371,7 @@
         <v>3.001371404115428</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="81"/>
       <c r="B15" s="34" t="s">
         <v>13</v>
@@ -3403,7 +3428,7 @@
         <v>2.9768279935895898</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="81"/>
       <c r="B16" s="34" t="s">
         <v>14</v>
@@ -3460,7 +3485,7 @@
         <v>2.4423431400467339</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="81"/>
       <c r="B17" s="34" t="s">
         <v>15</v>
@@ -3517,7 +3542,7 @@
         <v>2.8144326209735691</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="81" t="s">
         <v>85</v>
       </c>
@@ -3576,7 +3601,7 @@
         <v>3.5668052131556029</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="81"/>
       <c r="B19" s="48" t="s">
         <v>1</v>
@@ -3633,7 +3658,7 @@
         <v>4.0529896903791238</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="81"/>
       <c r="B20" s="48" t="s">
         <v>2</v>
@@ -3690,7 +3715,7 @@
         <v>4.3115733563210163</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="81"/>
       <c r="B21" s="48" t="s">
         <v>3</v>
@@ -3747,7 +3772,7 @@
         <v>3.629724341565661</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="81"/>
       <c r="B22" s="48" t="s">
         <v>4</v>
@@ -3804,7 +3829,7 @@
         <v>2.949193529531942</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="81"/>
       <c r="B23" s="48" t="s">
         <v>5</v>
@@ -3861,7 +3886,7 @@
         <v>2.5959713809084199</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="81"/>
       <c r="B24" s="48" t="s">
         <v>6</v>
@@ -3918,7 +3943,7 @@
         <v>2.930654020980263</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="81"/>
       <c r="B25" s="48" t="s">
         <v>7</v>
@@ -3975,7 +4000,7 @@
         <v>3.462886762272865</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="81"/>
       <c r="B26" s="48" t="s">
         <v>8</v>
@@ -4032,7 +4057,7 @@
         <v>3.1796263978546309</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="81"/>
       <c r="B27" s="48" t="s">
         <v>9</v>
@@ -4089,7 +4114,7 @@
         <v>3.1822678358086711</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="81"/>
       <c r="B28" s="48" t="s">
         <v>10</v>
@@ -4146,7 +4171,7 @@
         <v>3.07658862942833</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="81"/>
       <c r="B29" s="48" t="s">
         <v>11</v>
@@ -4203,7 +4228,7 @@
         <v>3.5861552161648351</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="81"/>
       <c r="B30" s="48" t="s">
         <v>12</v>
@@ -4260,7 +4285,7 @@
         <v>3.001371404115428</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="81"/>
       <c r="B31" s="48" t="s">
         <v>13</v>
@@ -4317,7 +4342,7 @@
         <v>2.9768279935895898</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="81"/>
       <c r="B32" s="48" t="s">
         <v>14</v>
@@ -4374,7 +4399,7 @@
         <v>2.4423431400467339</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="81"/>
       <c r="B33" s="48" t="s">
         <v>15</v>
@@ -4431,7 +4456,7 @@
         <v>2.8144326209735691</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="81" t="s">
         <v>99</v>
       </c>
@@ -4490,7 +4515,7 @@
         <v>3.5668052131556029</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="81"/>
       <c r="B35" s="70" t="s">
         <v>1</v>
@@ -4547,7 +4572,7 @@
         <v>4.0529896903791238</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="81"/>
       <c r="B36" s="70" t="s">
         <v>2</v>
@@ -4604,7 +4629,7 @@
         <v>4.3115733563210163</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="81"/>
       <c r="B37" s="70" t="s">
         <v>3</v>
@@ -4661,7 +4686,7 @@
         <v>3.629724341565661</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="81"/>
       <c r="B38" s="70" t="s">
         <v>4</v>
@@ -4718,7 +4743,7 @@
         <v>2.949193529531942</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="81"/>
       <c r="B39" s="70" t="s">
         <v>5</v>
@@ -4775,7 +4800,7 @@
         <v>2.5959713809084199</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="81"/>
       <c r="B40" s="70" t="s">
         <v>6</v>
@@ -4832,7 +4857,7 @@
         <v>2.930654020980263</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="81"/>
       <c r="B41" s="70" t="s">
         <v>7</v>
@@ -4889,7 +4914,7 @@
         <v>3.462886762272865</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="81"/>
       <c r="B42" s="70" t="s">
         <v>8</v>
@@ -4946,7 +4971,7 @@
         <v>3.1796263978546309</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="81"/>
       <c r="B43" s="70" t="s">
         <v>9</v>
@@ -5003,7 +5028,7 @@
         <v>3.1822678358086711</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="81"/>
       <c r="B44" s="70" t="s">
         <v>10</v>
@@ -5060,7 +5085,7 @@
         <v>3.07658862942833</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="81"/>
       <c r="B45" s="70" t="s">
         <v>11</v>
@@ -5117,7 +5142,7 @@
         <v>3.5861552161648351</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="81"/>
       <c r="B46" s="70" t="s">
         <v>12</v>
@@ -5174,7 +5199,7 @@
         <v>3.001371404115428</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="81"/>
       <c r="B47" s="70" t="s">
         <v>13</v>
@@ -5231,7 +5256,7 @@
         <v>2.9768279935895898</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="81"/>
       <c r="B48" s="70" t="s">
         <v>14</v>
@@ -5288,7 +5313,7 @@
         <v>2.4423431400467339</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="81"/>
       <c r="B49" s="70" t="s">
         <v>15</v>
@@ -5345,7 +5370,7 @@
         <v>2.8144326209735691</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="81" t="s">
         <v>100</v>
       </c>
@@ -5404,7 +5429,7 @@
         <v>3.5668052131556029</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="81"/>
       <c r="B51" s="70" t="s">
         <v>1</v>
@@ -5461,7 +5486,7 @@
         <v>4.0529896903791238</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="81"/>
       <c r="B52" s="70" t="s">
         <v>2</v>
@@ -5518,7 +5543,7 @@
         <v>4.3115733563210163</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="81"/>
       <c r="B53" s="70" t="s">
         <v>3</v>
@@ -5575,7 +5600,7 @@
         <v>3.629724341565661</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="81"/>
       <c r="B54" s="70" t="s">
         <v>4</v>
@@ -5632,7 +5657,7 @@
         <v>2.949193529531942</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="81"/>
       <c r="B55" s="70" t="s">
         <v>5</v>
@@ -5689,7 +5714,7 @@
         <v>2.5959713809084199</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="81"/>
       <c r="B56" s="70" t="s">
         <v>6</v>
@@ -5746,7 +5771,7 @@
         <v>2.930654020980263</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="81"/>
       <c r="B57" s="70" t="s">
         <v>7</v>
@@ -5803,7 +5828,7 @@
         <v>3.462886762272865</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="81"/>
       <c r="B58" s="70" t="s">
         <v>8</v>
@@ -5860,7 +5885,7 @@
         <v>3.1796263978546309</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="81"/>
       <c r="B59" s="70" t="s">
         <v>9</v>
@@ -5917,7 +5942,7 @@
         <v>3.1822678358086711</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="81"/>
       <c r="B60" s="70" t="s">
         <v>10</v>
@@ -5974,7 +5999,7 @@
         <v>3.07658862942833</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="81"/>
       <c r="B61" s="70" t="s">
         <v>11</v>
@@ -6031,7 +6056,7 @@
         <v>3.5861552161648351</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="81"/>
       <c r="B62" s="70" t="s">
         <v>12</v>
@@ -6088,7 +6113,7 @@
         <v>3.001371404115428</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="81"/>
       <c r="B63" s="70" t="s">
         <v>13</v>
@@ -6145,7 +6170,7 @@
         <v>2.9768279935895898</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="81"/>
       <c r="B64" s="70" t="s">
         <v>14</v>
@@ -6202,7 +6227,7 @@
         <v>2.4423431400467339</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="81"/>
       <c r="B65" s="70" t="s">
         <v>15</v>
@@ -6278,12 +6303,12 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -6306,7 +6331,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -6330,7 +6355,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>85</v>
       </c>
@@ -6356,7 +6381,7 @@
         <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>99</v>
       </c>
@@ -6382,7 +6407,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>100</v>
       </c>
@@ -6408,7 +6433,7 @@
         <v>5.4333333333333336</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="49"/>
     </row>
   </sheetData>
@@ -6424,21 +6449,21 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -6470,7 +6495,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
@@ -6502,7 +6527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>85</v>
       </c>
@@ -6534,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
@@ -6566,7 +6591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>100</v>
       </c>
@@ -6612,20 +6637,20 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -6657,7 +6682,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
@@ -6689,7 +6714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>85</v>
       </c>
@@ -6721,7 +6746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
@@ -6753,7 +6778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>100</v>
       </c>
@@ -6798,21 +6823,21 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="5"/>
-    <col min="9" max="9" width="10.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="5"/>
+    <col min="9" max="9" width="10.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -6844,7 +6869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>80</v>
       </c>
@@ -6876,7 +6901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>85</v>
       </c>
@@ -6908,7 +6933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>100</v>
       </c>
@@ -6940,7 +6965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>99</v>
       </c>
@@ -6985,20 +7010,20 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -7030,7 +7055,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
@@ -7062,7 +7087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>85</v>
       </c>
@@ -7094,7 +7119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>99</v>
       </c>
@@ -7126,7 +7151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>100</v>
       </c>
@@ -7171,20 +7196,20 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="32.21875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="23.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
         <v>17</v>
       </c>
@@ -7213,7 +7238,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="74" t="s">
         <v>80</v>
       </c>
@@ -7238,7 +7263,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="72"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>85</v>
       </c>
@@ -7263,7 +7288,7 @@
       <c r="H3" s="79"/>
       <c r="I3" s="80"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="74" t="s">
         <v>99</v>
       </c>
@@ -7288,7 +7313,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="72"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="76" t="s">
         <v>100</v>
       </c>
@@ -7323,29 +7348,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>17</v>
       </c>
@@ -7389,7 +7414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="82" t="s">
         <v>80</v>
       </c>
@@ -7430,7 +7455,7 @@
         <v>43906</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="83"/>
       <c r="B3" s="36" t="s">
         <v>71</v>
@@ -7469,7 +7494,7 @@
         <v>43913</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="83"/>
       <c r="B4" s="36" t="s">
         <v>72</v>
@@ -7508,7 +7533,7 @@
         <v>43977</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="83"/>
       <c r="B5" s="36" t="s">
         <v>73</v>
@@ -7547,7 +7572,7 @@
         <v>43992</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="83"/>
       <c r="B6" s="36" t="s">
         <v>74</v>
@@ -7583,7 +7608,7 @@
       </c>
       <c r="N6" s="39"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="83"/>
       <c r="B7" s="36" t="s">
         <v>77</v>
@@ -7617,7 +7642,7 @@
       <c r="M7" s="39"/>
       <c r="N7" s="39"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="83"/>
       <c r="B8" s="36" t="s">
         <v>79</v>
@@ -7651,7 +7676,7 @@
       <c r="M8" s="39"/>
       <c r="N8" s="46"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="84"/>
       <c r="B9" s="27" t="s">
         <v>75</v>
@@ -7685,7 +7710,7 @@
       <c r="M9" s="39"/>
       <c r="N9" s="22"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="85" t="s">
         <v>85</v>
       </c>
@@ -7726,7 +7751,7 @@
         <v>43908</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="86"/>
       <c r="B11" s="57" t="s">
         <v>71</v>
@@ -7765,7 +7790,7 @@
         <v>43914</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="86"/>
       <c r="B12" s="57" t="s">
         <v>72</v>
@@ -7804,7 +7829,7 @@
         <v>43949</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="86"/>
       <c r="B13" s="57" t="s">
         <v>73</v>
@@ -7843,7 +7868,7 @@
         <v>43972</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="86"/>
       <c r="B14" s="57" t="s">
         <v>74</v>
@@ -7879,7 +7904,7 @@
       </c>
       <c r="N14" s="59"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="86"/>
       <c r="B15" s="57" t="s">
         <v>77</v>
@@ -7913,7 +7938,7 @@
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="86"/>
       <c r="B16" s="57" t="s">
         <v>79</v>
@@ -7947,7 +7972,7 @@
       <c r="M16" s="59"/>
       <c r="N16" s="62"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="87"/>
       <c r="B17" s="63" t="s">
         <v>75</v>
@@ -7981,7 +8006,7 @@
       <c r="M17" s="69"/>
       <c r="N17" s="68"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="82" t="s">
         <v>99</v>
       </c>
@@ -8022,7 +8047,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="83"/>
       <c r="B19" s="36" t="s">
         <v>71</v>
@@ -8061,7 +8086,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="83"/>
       <c r="B20" s="36" t="s">
         <v>72</v>
@@ -8100,7 +8125,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="83"/>
       <c r="B21" s="36" t="s">
         <v>73</v>
@@ -8139,7 +8164,7 @@
         <v>43977</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="83"/>
       <c r="B22" s="36" t="s">
         <v>74</v>
@@ -8175,7 +8200,7 @@
       </c>
       <c r="N22" s="39"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="83"/>
       <c r="B23" s="36" t="s">
         <v>77</v>
@@ -8209,7 +8234,7 @@
       <c r="M23" s="39"/>
       <c r="N23" s="39"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="83"/>
       <c r="B24" s="36" t="s">
         <v>79</v>
@@ -8243,7 +8268,7 @@
       <c r="M24" s="39"/>
       <c r="N24" s="46"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="84"/>
       <c r="B25" s="27" t="s">
         <v>75</v>
@@ -8277,7 +8302,7 @@
       <c r="M25" s="39"/>
       <c r="N25" s="22"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="85" t="s">
         <v>100</v>
       </c>
@@ -8318,7 +8343,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="86"/>
       <c r="B27" s="57" t="s">
         <v>71</v>
@@ -8357,7 +8382,7 @@
         <v>43912</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="86"/>
       <c r="B28" s="57" t="s">
         <v>72</v>
@@ -8396,7 +8421,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="86"/>
       <c r="B29" s="57" t="s">
         <v>73</v>
@@ -8405,7 +8430,7 @@
         <v>83</v>
       </c>
       <c r="D29" s="58">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E29" s="61">
         <v>1</v>
@@ -8435,7 +8460,7 @@
         <v>43977</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="86"/>
       <c r="B30" s="57" t="s">
         <v>74</v>
@@ -8444,7 +8469,7 @@
         <v>84</v>
       </c>
       <c r="D30" s="58">
-        <v>0.28000000000000003</v>
+        <v>0.2</v>
       </c>
       <c r="E30" s="35">
         <v>1</v>
@@ -8471,7 +8496,7 @@
       </c>
       <c r="N30" s="59"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="86"/>
       <c r="B31" s="57" t="s">
         <v>77</v>
@@ -8505,7 +8530,7 @@
       <c r="M31" s="59"/>
       <c r="N31" s="59"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="86"/>
       <c r="B32" s="57" t="s">
         <v>79</v>
@@ -8539,7 +8564,7 @@
       <c r="M32" s="59"/>
       <c r="N32" s="62"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="87"/>
       <c r="B33" s="63" t="s">
         <v>75</v>
@@ -8590,20 +8615,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="9" max="9" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -8674,7 +8699,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -8732,7 +8757,7 @@
         <v>1000</v>
       </c>
       <c r="S2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="T2">
         <v>1</v>
@@ -8747,7 +8772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>85</v>
       </c>
@@ -8820,7 +8845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>99</v>
       </c>
@@ -8878,7 +8903,7 @@
         <v>1000</v>
       </c>
       <c r="S4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="T4">
         <v>1</v>
@@ -8893,7 +8918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>100</v>
       </c>
@@ -8951,7 +8976,7 @@
         <v>1000</v>
       </c>
       <c r="S5">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="T5">
         <v>1</v>

</xml_diff>